<commit_message>
alteracao layour matriz de confusao
</commit_message>
<xml_diff>
--- a/details-results/results_predict/dados_testes_detalhado.xlsx
+++ b/details-results/results_predict/dados_testes_detalhado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados dos testes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Explicações" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Dados dos testes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Explicações" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
correcao da matriz de confusão
</commit_message>
<xml_diff>
--- a/details-results/results_predict/dados_testes_detalhado.xlsx
+++ b/details-results/results_predict/dados_testes_detalhado.xlsx
@@ -513,43 +513,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9231</v>
+        <v>0.9615</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8889</v>
+        <v>0.9714</v>
       </c>
       <c r="D2" t="n">
+        <v>0.9722</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.9444</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.8889</v>
-      </c>
       <c r="H2" t="n">
-        <v>0.1111</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.0556</v>
       </c>
       <c r="J2" t="n">
         <v>8</v>
       </c>
       <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="N2" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionar mais imagens teste
</commit_message>
<xml_diff>
--- a/details-results/results_predict/dados_testes_detalhado.xlsx
+++ b/details-results/results_predict/dados_testes_detalhado.xlsx
@@ -513,43 +513,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8935999999999999</v>
+        <v>0.9177</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8996</v>
+        <v>0.9283</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8925999999999999</v>
+        <v>0.9137999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8704</v>
+        <v>0.9132</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9307</v>
+        <v>0.9439</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8545</v>
+        <v>0.8837</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1455</v>
+        <v>0.1163</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0693</v>
+        <v>0.0561</v>
       </c>
       <c r="J2" t="n">
-        <v>188</v>
+        <v>304</v>
       </c>
       <c r="K2" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L2" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="M2" t="n">
-        <v>215</v>
+        <v>421</v>
       </c>
       <c r="N2" t="n">
-        <v>451</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
envio das fotos e metricas igor 09112024
</commit_message>
<xml_diff>
--- a/details-results/results_predict/dados_testes_detalhado.xlsx
+++ b/details-results/results_predict/dados_testes_detalhado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados dos testes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Explicações" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Dados dos testes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Explicações" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -513,43 +513,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9177</v>
+        <v>0.9212</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9283</v>
+        <v>0.9301</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9137999999999999</v>
+        <v>0.9187</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9132</v>
+        <v>0.9196</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9439</v>
+        <v>0.9407</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8837</v>
+        <v>0.8966</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1163</v>
+        <v>0.1034</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0561</v>
+        <v>0.0593</v>
       </c>
       <c r="J2" t="n">
-        <v>304</v>
+        <v>373</v>
       </c>
       <c r="K2" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L2" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="M2" t="n">
-        <v>421</v>
+        <v>492</v>
       </c>
       <c r="N2" t="n">
-        <v>790</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>